<commit_message>
add results of small simulation 2
</commit_message>
<xml_diff>
--- a/SIMULATIONS/simulation_ideas_table.xlsx
+++ b/SIMULATIONS/simulation_ideas_table.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28429"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28623"/>
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Qba Liu\Documents\STUDIA\BIOINF_MASTER_BERLIN\MASTER_THESIS\SIMULATION_POLIGON\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Qba Liu\Documents\STUDIA\BIOINF_MASTER_BERLIN\MASTER_THESIS\MasterThesis_FUB\SIMULATIONS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0DED92D8-B095-4042-A31B-B2FC9DECBB3F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94FBAFE-10EC-4992-95CD-2575D39EE07D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{CC93E554-30B0-490D-8CFE-132AEC6C27E9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="94" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="32">
   <si>
     <t>description</t>
   </si>
@@ -299,6 +299,190 @@
     <t>aleternative pattern</t>
   </si>
   <si>
+    <t>Here I just want to look if the dimensionality impacts the power across the different covariance structures, while holding all other variables constant.</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>level1:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> covariance structure; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>level2:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sample size; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>level3:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> dimensionality; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>level4:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> variance; l</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">evel5: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>correlation</t>
+    </r>
+  </si>
+  <si>
+    <t>In this simulation I just want to see if there variance and the correlation have an effect on the power for different combinations of the covariance structure, sample size and dimensionality.</t>
+  </si>
+  <si>
+    <t>alpga</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>level1:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">  covariance structure;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> level2:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> columns under effect; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">level3: </t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>sample size</t>
+    </r>
+  </si>
+  <si>
+    <t>Here I just want to look at how the number of columns under effect influences the power across different covariance structures and sample sizes</t>
+  </si>
+  <si>
     <r>
       <rPr>
         <b/>
@@ -339,192 +523,8 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> dimensionality</t>
-    </r>
-  </si>
-  <si>
-    <t>Here I just want to look if the dimensionality impacts the power across the different covariance structures, while holding all other variables constant.</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>level1:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> covariance structure; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>level2:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> sample size; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>level3:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> dimensionality; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>level4:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> variance; l</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">evel5: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>correlation</t>
-    </r>
-  </si>
-  <si>
-    <t>In this simulation I just want to see if there variance and the correlation have an effect on the power for different combinations of the covariance structure, sample size and dimensionality.</t>
-  </si>
-  <si>
-    <t>alpga</t>
-  </si>
-  <si>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>level1:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">  covariance structure;</t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> level2:</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve"> columns under effect; </t>
-    </r>
-    <r>
-      <rPr>
-        <b/>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t xml:space="preserve">level3: </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="11"/>
-        <color theme="1"/>
-        <rFont val="Aptos Narrow"/>
-        <family val="2"/>
-        <scheme val="minor"/>
-      </rPr>
-      <t>sample size</t>
-    </r>
-  </si>
-  <si>
-    <t>Here I just want to look at how the number of columns under effect influences the power across different covariance structures and sample sizes</t>
+      <t xml:space="preserve"> dimensionality; level3: sample size</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -699,6 +699,51 @@
     <xf numFmtId="0" fontId="3" fillId="5" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -715,51 +760,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="1" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="2" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="4" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -1098,8 +1098,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E7E069-D7D9-4B6C-8EEC-D70EFC6B3529}">
   <dimension ref="A1:E64"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C50" workbookViewId="0">
-      <selection activeCell="H58" sqref="H58"/>
+    <sheetView tabSelected="1" topLeftCell="C26" workbookViewId="0">
+      <selection activeCell="E33" sqref="E33:E44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1130,7 +1130,7 @@
       </c>
     </row>
     <row r="2" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A2" s="25">
+      <c r="A2" s="26">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1139,107 +1139,107 @@
       <c r="C2" s="3" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="24" t="s">
+      <c r="D2" s="19" t="s">
         <v>12</v>
       </c>
-      <c r="E2" s="24"/>
+      <c r="E2" s="19"/>
     </row>
     <row r="3" spans="1:5" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="25"/>
+      <c r="A3" s="26"/>
       <c r="B3" s="4" t="s">
         <v>8</v>
       </c>
       <c r="C3" s="3" t="s">
         <v>5</v>
       </c>
-      <c r="D3" s="24"/>
-      <c r="E3" s="24"/>
+      <c r="D3" s="19"/>
+      <c r="E3" s="19"/>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A4" s="25"/>
+      <c r="A4" s="26"/>
       <c r="B4" s="3" t="s">
         <v>9</v>
       </c>
       <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="24"/>
-      <c r="E4" s="24"/>
+      <c r="D4" s="19"/>
+      <c r="E4" s="19"/>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A5" s="25"/>
+      <c r="A5" s="26"/>
       <c r="B5" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C5" s="3"/>
-      <c r="D5" s="24"/>
-      <c r="E5" s="24"/>
+      <c r="D5" s="19"/>
+      <c r="E5" s="19"/>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A6" s="25"/>
+      <c r="A6" s="26"/>
       <c r="B6" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C6" s="3"/>
-      <c r="D6" s="24"/>
-      <c r="E6" s="24"/>
+      <c r="D6" s="19"/>
+      <c r="E6" s="19"/>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A7" s="25"/>
+      <c r="A7" s="26"/>
       <c r="B7" s="3" t="s">
         <v>15</v>
       </c>
       <c r="C7" s="3"/>
-      <c r="D7" s="24"/>
-      <c r="E7" s="24"/>
+      <c r="D7" s="19"/>
+      <c r="E7" s="19"/>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A8" s="25"/>
+      <c r="A8" s="26"/>
       <c r="B8" s="3" t="s">
         <v>17</v>
       </c>
       <c r="C8" s="3"/>
-      <c r="D8" s="24"/>
-      <c r="E8" s="24"/>
+      <c r="D8" s="19"/>
+      <c r="E8" s="19"/>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A9" s="25"/>
+      <c r="A9" s="26"/>
       <c r="B9" s="3" t="s">
         <v>18</v>
       </c>
       <c r="C9" s="3"/>
-      <c r="D9" s="24"/>
-      <c r="E9" s="24"/>
+      <c r="D9" s="19"/>
+      <c r="E9" s="19"/>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A10" s="25"/>
+      <c r="A10" s="26"/>
       <c r="B10" s="3" t="s">
         <v>19</v>
       </c>
       <c r="C10" s="3"/>
-      <c r="D10" s="24"/>
-      <c r="E10" s="24"/>
+      <c r="D10" s="19"/>
+      <c r="E10" s="19"/>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A11" s="25"/>
+      <c r="A11" s="26"/>
       <c r="B11" s="3" t="s">
         <v>16</v>
       </c>
       <c r="C11" s="3"/>
-      <c r="D11" s="24"/>
-      <c r="E11" s="24"/>
+      <c r="D11" s="19"/>
+      <c r="E11" s="19"/>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A12" s="25"/>
+      <c r="A12" s="26"/>
       <c r="B12" s="3" t="s">
         <v>10</v>
       </c>
       <c r="C12" s="3"/>
-      <c r="D12" s="24"/>
-      <c r="E12" s="24"/>
+      <c r="D12" s="19"/>
+      <c r="E12" s="19"/>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A13" s="12">
+      <c r="A13" s="27">
         <v>2</v>
       </c>
       <c r="B13" s="5" t="s">
@@ -1254,7 +1254,7 @@
       <c r="E13" s="7"/>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A14" s="13"/>
+      <c r="A14" s="28"/>
       <c r="B14" s="6" t="s">
         <v>18</v>
       </c>
@@ -1265,7 +1265,7 @@
       <c r="E14" s="8"/>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A15" s="13"/>
+      <c r="A15" s="28"/>
       <c r="B15" s="6" t="s">
         <v>6</v>
       </c>
@@ -1274,7 +1274,7 @@
       <c r="E15" s="8"/>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A16" s="13"/>
+      <c r="A16" s="28"/>
       <c r="B16" s="6" t="s">
         <v>13</v>
       </c>
@@ -1283,7 +1283,7 @@
       <c r="E16" s="8"/>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A17" s="13"/>
+      <c r="A17" s="28"/>
       <c r="B17" s="5" t="s">
         <v>14</v>
       </c>
@@ -1292,7 +1292,7 @@
       <c r="E17" s="8"/>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A18" s="13"/>
+      <c r="A18" s="28"/>
       <c r="B18" s="5" t="s">
         <v>9</v>
       </c>
@@ -1301,7 +1301,7 @@
       <c r="E18" s="8"/>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A19" s="13"/>
+      <c r="A19" s="28"/>
       <c r="B19" s="5" t="s">
         <v>11</v>
       </c>
@@ -1310,7 +1310,7 @@
       <c r="E19" s="8"/>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A20" s="13"/>
+      <c r="A20" s="28"/>
       <c r="B20" s="5" t="s">
         <v>16</v>
       </c>
@@ -1319,7 +1319,7 @@
       <c r="E20" s="8"/>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A21" s="14"/>
+      <c r="A21" s="29"/>
       <c r="B21" s="5" t="s">
         <v>19</v>
       </c>
@@ -1328,7 +1328,7 @@
       <c r="E21" s="9"/>
     </row>
     <row r="22" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A22" s="18">
+      <c r="A22" s="20">
         <v>3</v>
       </c>
       <c r="B22" s="10" t="s">
@@ -1337,105 +1337,105 @@
       <c r="C22" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D22" s="21" t="s">
+      <c r="D22" s="23" t="s">
         <v>23</v>
       </c>
-      <c r="E22" s="21"/>
+      <c r="E22" s="23"/>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A23" s="19"/>
+      <c r="A23" s="21"/>
       <c r="B23" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C23" s="10" t="s">
         <v>6</v>
       </c>
-      <c r="D23" s="22"/>
-      <c r="E23" s="22"/>
+      <c r="D23" s="24"/>
+      <c r="E23" s="24"/>
     </row>
     <row r="24" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A24" s="19"/>
+      <c r="A24" s="21"/>
       <c r="B24" s="10"/>
       <c r="C24" s="10" t="s">
         <v>20</v>
       </c>
-      <c r="D24" s="22"/>
-      <c r="E24" s="22"/>
+      <c r="D24" s="24"/>
+      <c r="E24" s="24"/>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A25" s="19"/>
+      <c r="A25" s="21"/>
       <c r="B25" s="11"/>
       <c r="C25" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D25" s="22"/>
-      <c r="E25" s="22"/>
+      <c r="D25" s="24"/>
+      <c r="E25" s="24"/>
     </row>
     <row r="26" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A26" s="19"/>
+      <c r="A26" s="21"/>
       <c r="B26" s="10" t="s">
         <v>13</v>
       </c>
       <c r="C26" s="10"/>
-      <c r="D26" s="22"/>
-      <c r="E26" s="22"/>
+      <c r="D26" s="24"/>
+      <c r="E26" s="24"/>
     </row>
     <row r="27" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A27" s="19"/>
+      <c r="A27" s="21"/>
       <c r="B27" s="10" t="s">
         <v>14</v>
       </c>
       <c r="C27" s="10"/>
-      <c r="D27" s="22"/>
-      <c r="E27" s="22"/>
+      <c r="D27" s="24"/>
+      <c r="E27" s="24"/>
     </row>
     <row r="28" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A28" s="19"/>
+      <c r="A28" s="21"/>
       <c r="B28" s="10" t="s">
         <v>15</v>
       </c>
       <c r="C28" s="10"/>
-      <c r="D28" s="22"/>
-      <c r="E28" s="22"/>
+      <c r="D28" s="24"/>
+      <c r="E28" s="24"/>
     </row>
     <row r="29" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A29" s="19"/>
+      <c r="A29" s="21"/>
       <c r="B29" s="10" t="s">
         <v>17</v>
       </c>
       <c r="C29" s="10"/>
-      <c r="D29" s="22"/>
-      <c r="E29" s="22"/>
+      <c r="D29" s="24"/>
+      <c r="E29" s="24"/>
     </row>
     <row r="30" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A30" s="19"/>
+      <c r="A30" s="21"/>
       <c r="B30" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C30" s="10"/>
-      <c r="D30" s="22"/>
-      <c r="E30" s="22"/>
+      <c r="D30" s="24"/>
+      <c r="E30" s="24"/>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A31" s="19"/>
+      <c r="A31" s="21"/>
       <c r="B31" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C31" s="10"/>
-      <c r="D31" s="22"/>
-      <c r="E31" s="22"/>
+      <c r="D31" s="24"/>
+      <c r="E31" s="24"/>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A32" s="20"/>
+      <c r="A32" s="22"/>
       <c r="B32" s="10" t="s">
         <v>9</v>
       </c>
       <c r="C32" s="10"/>
-      <c r="D32" s="23"/>
-      <c r="E32" s="23"/>
+      <c r="D32" s="25"/>
+      <c r="E32" s="25"/>
     </row>
     <row r="33" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A33" s="12">
+      <c r="A33" s="27">
         <v>4</v>
       </c>
       <c r="B33" s="5" t="s">
@@ -1444,116 +1444,118 @@
       <c r="C33" s="5" t="s">
         <v>5</v>
       </c>
-      <c r="D33" s="15" t="s">
+      <c r="D33" s="30" t="s">
+        <v>31</v>
+      </c>
+      <c r="E33" s="30" t="s">
         <v>25</v>
       </c>
-      <c r="E33" s="15" t="s">
-        <v>26</v>
-      </c>
     </row>
     <row r="34" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A34" s="13"/>
+      <c r="A34" s="28"/>
       <c r="B34" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C34" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="D34" s="16"/>
-      <c r="E34" s="16"/>
+      <c r="D34" s="31"/>
+      <c r="E34" s="31"/>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A35" s="13"/>
+      <c r="A35" s="28"/>
       <c r="B35" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="C35" s="5"/>
-      <c r="D35" s="16"/>
-      <c r="E35" s="16"/>
+      <c r="C35" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="D35" s="31"/>
+      <c r="E35" s="31"/>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A36" s="13"/>
+      <c r="A36" s="28"/>
       <c r="B36" s="5" t="s">
         <v>11</v>
       </c>
       <c r="C36" s="5"/>
-      <c r="D36" s="16"/>
-      <c r="E36" s="16"/>
+      <c r="D36" s="31"/>
+      <c r="E36" s="31"/>
     </row>
     <row r="37" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A37" s="13"/>
+      <c r="A37" s="28"/>
       <c r="B37" s="5" t="s">
         <v>13</v>
       </c>
       <c r="C37" s="5"/>
-      <c r="D37" s="16"/>
-      <c r="E37" s="16"/>
+      <c r="D37" s="31"/>
+      <c r="E37" s="31"/>
     </row>
     <row r="38" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A38" s="13"/>
+      <c r="A38" s="28"/>
       <c r="B38" s="5" t="s">
         <v>14</v>
       </c>
       <c r="C38" s="5"/>
-      <c r="D38" s="16"/>
-      <c r="E38" s="16"/>
+      <c r="D38" s="31"/>
+      <c r="E38" s="31"/>
     </row>
     <row r="39" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A39" s="13"/>
+      <c r="A39" s="28"/>
       <c r="B39" s="5" t="s">
         <v>15</v>
       </c>
       <c r="C39" s="5"/>
-      <c r="D39" s="16"/>
-      <c r="E39" s="16"/>
+      <c r="D39" s="31"/>
+      <c r="E39" s="31"/>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A40" s="13"/>
+      <c r="A40" s="28"/>
       <c r="B40" s="5" t="s">
         <v>19</v>
       </c>
       <c r="C40" s="5"/>
-      <c r="D40" s="16"/>
-      <c r="E40" s="16"/>
+      <c r="D40" s="31"/>
+      <c r="E40" s="31"/>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A41" s="13"/>
+      <c r="A41" s="28"/>
       <c r="B41" s="5" t="s">
         <v>17</v>
       </c>
       <c r="C41" s="5"/>
-      <c r="D41" s="16"/>
-      <c r="E41" s="16"/>
+      <c r="D41" s="31"/>
+      <c r="E41" s="31"/>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A42" s="13"/>
+      <c r="A42" s="28"/>
       <c r="B42" s="5" t="s">
         <v>16</v>
       </c>
       <c r="C42" s="5"/>
-      <c r="D42" s="16"/>
-      <c r="E42" s="16"/>
+      <c r="D42" s="31"/>
+      <c r="E42" s="31"/>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A43" s="13"/>
+      <c r="A43" s="28"/>
       <c r="B43" s="5" t="s">
         <v>18</v>
       </c>
       <c r="C43" s="5"/>
-      <c r="D43" s="16"/>
-      <c r="E43" s="16"/>
+      <c r="D43" s="31"/>
+      <c r="E43" s="31"/>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A44" s="14"/>
+      <c r="A44" s="29"/>
       <c r="B44" s="5" t="s">
         <v>24</v>
       </c>
       <c r="C44" s="5"/>
-      <c r="D44" s="17"/>
-      <c r="E44" s="17"/>
+      <c r="D44" s="32"/>
+      <c r="E44" s="32"/>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A45" s="18">
+      <c r="A45" s="20">
         <v>5</v>
       </c>
       <c r="B45" s="10" t="s">
@@ -1562,203 +1564,203 @@
       <c r="C45" s="10" t="s">
         <v>5</v>
       </c>
-      <c r="D45" s="21" t="s">
+      <c r="D45" s="23" t="s">
+        <v>26</v>
+      </c>
+      <c r="E45" s="23" t="s">
         <v>27</v>
       </c>
-      <c r="E45" s="21" t="s">
-        <v>28</v>
-      </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A46" s="19"/>
+      <c r="A46" s="21"/>
       <c r="B46" s="10" t="s">
         <v>7</v>
       </c>
       <c r="C46" s="10" t="s">
         <v>13</v>
       </c>
-      <c r="D46" s="22"/>
-      <c r="E46" s="22"/>
+      <c r="D46" s="24"/>
+      <c r="E46" s="24"/>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A47" s="19"/>
+      <c r="A47" s="21"/>
       <c r="B47" s="10" t="s">
         <v>11</v>
       </c>
       <c r="C47" s="10" t="s">
         <v>14</v>
       </c>
-      <c r="D47" s="22"/>
-      <c r="E47" s="22"/>
+      <c r="D47" s="24"/>
+      <c r="E47" s="24"/>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A48" s="19"/>
+      <c r="A48" s="21"/>
       <c r="B48" s="10" t="s">
         <v>15</v>
       </c>
       <c r="C48" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="D48" s="22"/>
-      <c r="E48" s="22"/>
+      <c r="D48" s="24"/>
+      <c r="E48" s="24"/>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A49" s="19"/>
+      <c r="A49" s="21"/>
       <c r="B49" s="10" t="s">
         <v>19</v>
       </c>
       <c r="C49" s="10" t="s">
         <v>4</v>
       </c>
-      <c r="D49" s="22"/>
-      <c r="E49" s="22"/>
+      <c r="D49" s="24"/>
+      <c r="E49" s="24"/>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A50" s="19"/>
+      <c r="A50" s="21"/>
       <c r="B50" s="10" t="s">
         <v>17</v>
       </c>
       <c r="C50" s="10"/>
-      <c r="D50" s="22"/>
-      <c r="E50" s="22"/>
+      <c r="D50" s="24"/>
+      <c r="E50" s="24"/>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A51" s="19"/>
+      <c r="A51" s="21"/>
       <c r="B51" s="10" t="s">
         <v>16</v>
       </c>
       <c r="C51" s="10"/>
-      <c r="D51" s="22"/>
-      <c r="E51" s="22"/>
+      <c r="D51" s="24"/>
+      <c r="E51" s="24"/>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A52" s="19"/>
+      <c r="A52" s="21"/>
       <c r="B52" s="10" t="s">
         <v>18</v>
       </c>
       <c r="C52" s="10"/>
-      <c r="D52" s="22"/>
-      <c r="E52" s="22"/>
+      <c r="D52" s="24"/>
+      <c r="E52" s="24"/>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A53" s="19"/>
+      <c r="A53" s="21"/>
       <c r="B53" s="10" t="s">
         <v>4</v>
       </c>
       <c r="C53" s="10"/>
-      <c r="D53" s="22"/>
-      <c r="E53" s="22"/>
+      <c r="D53" s="24"/>
+      <c r="E53" s="24"/>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A54" s="20"/>
+      <c r="A54" s="22"/>
       <c r="B54" s="10" t="s">
         <v>10</v>
       </c>
       <c r="C54" s="10"/>
-      <c r="D54" s="23"/>
-      <c r="E54" s="23"/>
+      <c r="D54" s="25"/>
+      <c r="E54" s="25"/>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A55" s="26">
+      <c r="A55" s="13">
         <v>6</v>
       </c>
-      <c r="B55" s="27" t="s">
+      <c r="B55" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C55" s="27" t="s">
+      <c r="C55" s="12" t="s">
         <v>11</v>
       </c>
-      <c r="D55" s="28" t="s">
+      <c r="D55" s="16" t="s">
+        <v>29</v>
+      </c>
+      <c r="E55" s="16" t="s">
         <v>30</v>
       </c>
-      <c r="E55" s="28" t="s">
-        <v>31</v>
-      </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A56" s="29"/>
-      <c r="B56" s="27" t="s">
+      <c r="A56" s="14"/>
+      <c r="B56" s="12" t="s">
         <v>7</v>
       </c>
-      <c r="C56" s="27" t="s">
+      <c r="C56" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="D56" s="30"/>
-      <c r="E56" s="30"/>
+      <c r="D56" s="17"/>
+      <c r="E56" s="17"/>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A57" s="29"/>
-      <c r="B57" s="27" t="s">
+      <c r="A57" s="14"/>
+      <c r="B57" s="12" t="s">
         <v>15</v>
       </c>
-      <c r="C57" s="27" t="s">
+      <c r="C57" s="12" t="s">
         <v>4</v>
       </c>
-      <c r="D57" s="30"/>
-      <c r="E57" s="30"/>
+      <c r="D57" s="17"/>
+      <c r="E57" s="17"/>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A58" s="29"/>
-      <c r="B58" s="27" t="s">
-        <v>29</v>
-      </c>
-      <c r="C58" s="27"/>
-      <c r="D58" s="30"/>
-      <c r="E58" s="30"/>
+      <c r="A58" s="14"/>
+      <c r="B58" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="C58" s="12"/>
+      <c r="D58" s="17"/>
+      <c r="E58" s="17"/>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A59" s="29"/>
-      <c r="B59" s="27" t="s">
+      <c r="A59" s="14"/>
+      <c r="B59" s="12" t="s">
         <v>13</v>
       </c>
-      <c r="C59" s="27"/>
-      <c r="D59" s="30"/>
-      <c r="E59" s="30"/>
+      <c r="C59" s="12"/>
+      <c r="D59" s="17"/>
+      <c r="E59" s="17"/>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A60" s="29"/>
-      <c r="B60" s="27" t="s">
+      <c r="A60" s="14"/>
+      <c r="B60" s="12" t="s">
         <v>9</v>
       </c>
-      <c r="C60" s="27"/>
-      <c r="D60" s="30"/>
-      <c r="E60" s="30"/>
+      <c r="C60" s="12"/>
+      <c r="D60" s="17"/>
+      <c r="E60" s="17"/>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A61" s="29"/>
-      <c r="B61" s="27" t="s">
+      <c r="A61" s="14"/>
+      <c r="B61" s="12" t="s">
         <v>6</v>
       </c>
-      <c r="C61" s="27"/>
-      <c r="D61" s="30"/>
-      <c r="E61" s="30"/>
+      <c r="C61" s="12"/>
+      <c r="D61" s="17"/>
+      <c r="E61" s="17"/>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A62" s="29"/>
-      <c r="B62" s="27" t="s">
+      <c r="A62" s="14"/>
+      <c r="B62" s="12" t="s">
         <v>17</v>
       </c>
-      <c r="C62" s="27"/>
-      <c r="D62" s="30"/>
-      <c r="E62" s="30"/>
+      <c r="C62" s="12"/>
+      <c r="D62" s="17"/>
+      <c r="E62" s="17"/>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A63" s="29"/>
-      <c r="B63" s="27" t="s">
+      <c r="A63" s="14"/>
+      <c r="B63" s="12" t="s">
         <v>10</v>
       </c>
-      <c r="C63" s="27"/>
-      <c r="D63" s="30"/>
-      <c r="E63" s="30"/>
+      <c r="C63" s="12"/>
+      <c r="D63" s="17"/>
+      <c r="E63" s="17"/>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.35">
-      <c r="A64" s="31"/>
-      <c r="B64" s="27" t="s">
+      <c r="A64" s="15"/>
+      <c r="B64" s="12" t="s">
         <v>18</v>
       </c>
-      <c r="C64" s="27"/>
-      <c r="D64" s="32"/>
-      <c r="E64" s="32"/>
+      <c r="C64" s="12"/>
+      <c r="D64" s="18"/>
+      <c r="E64" s="18"/>
     </row>
   </sheetData>
   <mergeCells count="16">

</xml_diff>

<commit_message>
add new simulation ideas
</commit_message>
<xml_diff>
--- a/SIMULATIONS/simulation_ideas_table.xlsx
+++ b/SIMULATIONS/simulation_ideas_table.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Qba Liu\Documents\STUDIA\BIOINF_MASTER_BERLIN\MASTER_THESIS\MasterThesis_FUB\SIMULATIONS\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E94FBAFE-10EC-4992-95CD-2575D39EE07D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9319F238-9396-4BC6-A62F-0D49A0C2A111}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{CC93E554-30B0-490D-8CFE-132AEC6C27E9}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="95" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="34">
   <si>
     <t>description</t>
   </si>
@@ -523,7 +523,158 @@
         <family val="2"/>
         <scheme val="minor"/>
       </rPr>
-      <t xml:space="preserve"> dimensionality; level3: sample size</t>
+      <t xml:space="preserve"> dimensionality; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>level3:</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> sample size</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>level1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: covariance structure; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>level2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: correlation; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>level 3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: sample size</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>level1</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: covariance structure;</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve"> level2</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t xml:space="preserve">: variance; </t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>level 3</t>
+    </r>
+    <r>
+      <rPr>
+        <sz val="11"/>
+        <color theme="1"/>
+        <rFont val="Aptos Narrow"/>
+        <family val="2"/>
+        <scheme val="minor"/>
+      </rPr>
+      <t>: sample size</t>
     </r>
   </si>
 </sst>
@@ -1096,10 +1247,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D2E7E069-D7D9-4B6C-8EEC-D70EFC6B3529}">
-  <dimension ref="A1:E64"/>
+  <dimension ref="A1:E80"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C26" workbookViewId="0">
-      <selection activeCell="E33" sqref="E33:E44"/>
+    <sheetView tabSelected="1" topLeftCell="A63" workbookViewId="0">
+      <selection activeCell="D65" sqref="D65:D72"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1762,8 +1913,138 @@
       <c r="D64" s="18"/>
       <c r="E64" s="18"/>
     </row>
+    <row r="65" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A65" s="20">
+        <v>7</v>
+      </c>
+      <c r="B65" s="20"/>
+      <c r="C65" s="20"/>
+      <c r="D65" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="E65" s="20"/>
+    </row>
+    <row r="66" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A66" s="21"/>
+      <c r="B66" s="21"/>
+      <c r="C66" s="21"/>
+      <c r="D66" s="21"/>
+      <c r="E66" s="21"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A67" s="21"/>
+      <c r="B67" s="21"/>
+      <c r="C67" s="21"/>
+      <c r="D67" s="21"/>
+      <c r="E67" s="21"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A68" s="21"/>
+      <c r="B68" s="21"/>
+      <c r="C68" s="21"/>
+      <c r="D68" s="21"/>
+      <c r="E68" s="21"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A69" s="21"/>
+      <c r="B69" s="21"/>
+      <c r="C69" s="21"/>
+      <c r="D69" s="21"/>
+      <c r="E69" s="21"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A70" s="21"/>
+      <c r="B70" s="21"/>
+      <c r="C70" s="21"/>
+      <c r="D70" s="21"/>
+      <c r="E70" s="21"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A71" s="21"/>
+      <c r="B71" s="21"/>
+      <c r="C71" s="21"/>
+      <c r="D71" s="21"/>
+      <c r="E71" s="21"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A72" s="21"/>
+      <c r="B72" s="21"/>
+      <c r="C72" s="21"/>
+      <c r="D72" s="21"/>
+      <c r="E72" s="21"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A73" s="16">
+        <v>8</v>
+      </c>
+      <c r="B73" s="16"/>
+      <c r="C73" s="16"/>
+      <c r="D73" s="16" t="s">
+        <v>33</v>
+      </c>
+      <c r="E73" s="16"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A74" s="17"/>
+      <c r="B74" s="17"/>
+      <c r="C74" s="17"/>
+      <c r="D74" s="17"/>
+      <c r="E74" s="17"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A75" s="17"/>
+      <c r="B75" s="17"/>
+      <c r="C75" s="17"/>
+      <c r="D75" s="17"/>
+      <c r="E75" s="17"/>
+    </row>
+    <row r="76" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A76" s="17"/>
+      <c r="B76" s="17"/>
+      <c r="C76" s="17"/>
+      <c r="D76" s="17"/>
+      <c r="E76" s="17"/>
+    </row>
+    <row r="77" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A77" s="17"/>
+      <c r="B77" s="17"/>
+      <c r="C77" s="17"/>
+      <c r="D77" s="17"/>
+      <c r="E77" s="17"/>
+    </row>
+    <row r="78" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A78" s="17"/>
+      <c r="B78" s="17"/>
+      <c r="C78" s="17"/>
+      <c r="D78" s="17"/>
+      <c r="E78" s="17"/>
+    </row>
+    <row r="79" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A79" s="17"/>
+      <c r="B79" s="17"/>
+      <c r="C79" s="17"/>
+      <c r="D79" s="17"/>
+      <c r="E79" s="17"/>
+    </row>
+    <row r="80" spans="1:5" x14ac:dyDescent="0.35">
+      <c r="A80" s="17"/>
+      <c r="B80" s="17"/>
+      <c r="C80" s="17"/>
+      <c r="D80" s="17"/>
+      <c r="E80" s="17"/>
+    </row>
   </sheetData>
-  <mergeCells count="16">
+  <mergeCells count="26">
+    <mergeCell ref="A73:A80"/>
+    <mergeCell ref="B73:B80"/>
+    <mergeCell ref="C73:C80"/>
+    <mergeCell ref="D73:D80"/>
+    <mergeCell ref="E73:E80"/>
+    <mergeCell ref="A65:A72"/>
+    <mergeCell ref="B65:B72"/>
+    <mergeCell ref="C65:C72"/>
+    <mergeCell ref="D65:D72"/>
+    <mergeCell ref="E65:E72"/>
     <mergeCell ref="A55:A64"/>
     <mergeCell ref="D55:D64"/>
     <mergeCell ref="E55:E64"/>

</xml_diff>